<commit_message>
Added theory on emergency management and  and plan for transport
</commit_message>
<xml_diff>
--- a/General/Ingmar/Transport.xlsx
+++ b/General/Ingmar/Transport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
   <si>
     <t>Optie altijd voordeel</t>
   </si>
@@ -111,13 +111,19 @@
   </si>
   <si>
     <t>Brandstofprijs</t>
+  </si>
+  <si>
+    <t>Optie boete</t>
+  </si>
+  <si>
+    <t>Goedkoopst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +153,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +210,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -195,20 +242,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,518 +574,626 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E49C9C-CAF0-421A-ACF5-EF411EED135E}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="2">
         <f>50/12</f>
         <v>4.166666666666667</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="2">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="2">
+        <f>2*97</f>
+        <v>194</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="2">
         <v>333</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="2">
+      <c r="R3" s="2">
         <f>60*26+250</f>
         <v>1810</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="3">
         <f>-50/12</f>
         <v>-4.166666666666667</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="3">
         <f>-50/12</f>
         <v>-4.166666666666667</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="3">
         <f>-50/12</f>
         <v>-4.166666666666667</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="2">
+      <c r="R4" s="2">
         <v>7.65</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N5" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="2">
+      <c r="R5" s="2">
         <v>1.65</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N6" t="s">
+      <c r="Q6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="2">
+      <c r="R6" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="2">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="2">
         <v>20</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L7" s="2">
         <v>20</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="2">
+      <c r="R7" s="2">
         <v>1500</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="2">
         <v>0.2</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="N8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2">
         <v>5.7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="2">
         <f>C9*(1-F8)</f>
         <v>5.7</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="2">
         <f>C9*(1-I8)</f>
         <v>4.5600000000000005</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L9" s="2">
-        <f>F9*(1-L8)</f>
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
+        <f>C9*(1-L8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" s="2">
+        <f>F9*(1-O8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="1">
-        <f>O7/12</f>
+      <c r="R9" s="4">
+        <f>R7/12</f>
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2">
         <v>5.03</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="2">
         <f>C10*(1-F8)</f>
         <v>5.03</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="2">
         <f>C10*(1-I8)</f>
         <v>4.024</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L10" s="2">
-        <f>F10*(1-L8)</f>
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
+        <f>C10*(1-L8)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="2">
+        <f>F10*(1-O8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O10" s="2">
+      <c r="R10" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="2">
         <v>6</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="2">
         <v>6</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="2">
         <v>6</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L11" s="2">
         <v>6</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="2">
+      <c r="R11" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="2">
         <v>0.4</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="2">
         <v>0.4</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L12" s="2">
         <v>1</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O12" s="2">
+      <c r="R12" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="2">
         <v>5.7</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="2">
         <f>C13*(1-F12)</f>
         <v>3.42</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="2">
         <f>C13*(1-I12)</f>
         <v>3.42</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L13" s="2">
-        <f>F13*(1-L12)</f>
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
+        <f>C13*(1-L12)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" s="2">
+        <f>F13*(1-O12)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O13" s="1">
-        <f>O3*O4*O5/100</f>
+      <c r="R13" s="4">
+        <f>R3*R4*R5/100</f>
         <v>228.46724999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="2">
         <v>5.03</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="2">
         <f>C14*(1-F12)</f>
         <v>3.0180000000000002</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I14" s="2">
         <f>C14*(1-I12)</f>
         <v>3.0180000000000002</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L14" s="2">
-        <f>F14*(1-L12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+        <f>C14*(1-L12)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="2">
+        <f>F14*(1-O12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <f>(C7+C11)*0.5*10</f>
         <v>130</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="4">
         <f>(F7+F11)*0.5*10</f>
         <v>130</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="4">
         <f>(I7+I11)*0.5*10</f>
         <v>130</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="4">
         <f>(L7+L11)*0.5*10</f>
         <v>130</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="N16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="4">
+        <f>(O7+O11)*0.5*10</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <f>C7*(C9+C10)+C11*(C13+C14)+C3+C4</f>
         <v>278.98</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="4">
         <f>F7*(F9+F10)+F11*(F13+F14)+F3+F4</f>
         <v>253.22800000000004</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="4">
         <f>I7*(I9+I10)+I11*(I13+I14)+I3+I4</f>
         <v>226.14133333333334</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="4">
         <f>L7*(L9+L10)+L11*(L13+L14)+L3+L4</f>
+        <v>194</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="4">
+        <f>O7*(O9+O10)+O11*(O13+O14)+O3+O4</f>
         <v>328.83333333333331</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>50</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="4">
         <v>30</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="4">
         <v>30</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="L18" s="4">
+        <v>30</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <f>C18+C17+C16</f>
         <v>458.98</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="4">
         <f>F18+F17+F16</f>
         <v>413.22800000000007</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="4">
         <f>I18+I17+I16</f>
         <v>386.14133333333336</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="4">
         <f>L18+L17+L16</f>
+        <v>354</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="4">
+        <f>O18+O17+O16</f>
         <v>458.83333333333331</v>
       </c>
-      <c r="N20" t="s">
+      <c r="Q20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O20" s="1">
-        <f>SUM(O9:O13)</f>
+      <c r="R20" s="4">
+        <f>SUM(R9:R13)</f>
         <v>513.46724999999992</v>
       </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="K22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>